<commit_message>
add test by chatgtp
</commit_message>
<xml_diff>
--- a/bin/config/xlsx/conditions.xlsx
+++ b/bin/config/xlsx/conditions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21360" windowHeight="10620"/>
+    <workbookView windowWidth="21220" windowHeight="17160"/>
   </bookViews>
   <sheets>
     <sheet name="condition" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">condition!$B:$B</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,7 +56,7 @@
     <t>amount</t>
   </si>
   <si>
-    <t>operation</t>
+    <t>comparison</t>
   </si>
   <si>
     <t>design</t>
@@ -118,54 +131,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,14 +160,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,6 +199,21 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -279,7 +264,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,49 +300,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,121 +438,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,21 +491,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -532,6 +523,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,148 +596,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -739,59 +745,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1064,13 +1070,13 @@
   <sheetPr/>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="10" max="10" width="13.6272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>